<commit_message>
LHC leva em conta variáveis discretas agora
</commit_message>
<xml_diff>
--- a/NewInputVariables.xlsx
+++ b/NewInputVariables.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,24 +478,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tank Diameter</t>
+          <t>Viscosity</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>77.5</v>
+        <v>800</v>
       </c>
       <c r="C2" t="n">
-        <v>11.47980278080471</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>882.2426813475736</v>
       </c>
       <c r="E2" t="n">
-        <v>55</v>
+        <v>717.7573186524264</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -506,24 +506,24 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tank Level</t>
+          <t>Densidade</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>1500</v>
       </c>
       <c r="C3" t="n">
-        <v>3.571494198472578</v>
+        <v>194.1122415647322</v>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>2000</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -534,51 +534,53 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Viscosity</t>
+          <t>Numero de Pratos</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>897.9981992270027</v>
+        <v>15</v>
       </c>
       <c r="E4" t="n">
-        <v>702.0018007729973</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
       <c r="G4" t="n">
         <v>0.95</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Continuous</t>
+          <t>Discrete</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Number of Impellers</t>
+          <t>Discreto 2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5102134569246539</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
         <v>3</v>
       </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G5" t="n">
         <v>0.95</v>
@@ -586,118 +588,6 @@
       <c r="H5" t="inlineStr">
         <is>
           <t>Discrete</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Impeller 1 Angle</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3.826600926934905</v>
-      </c>
-      <c r="D6" t="n">
-        <v>20</v>
-      </c>
-      <c r="E6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Continuous</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Impeller 2 Angle</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3.826600926934905</v>
-      </c>
-      <c r="D7" t="n">
-        <v>20</v>
-      </c>
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Continuous</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Impeller 3 Angle</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>3.826600926934905</v>
-      </c>
-      <c r="D8" t="n">
-        <v>20</v>
-      </c>
-      <c r="E8" t="n">
-        <v>5</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Continuous</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Densidade</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="C9" t="n">
-        <v>255.106728462327</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Continuous</t>
         </is>
       </c>
     </row>

</xml_diff>